<commit_message>
Allow spaces at the end of hearing time
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/data/non-strategic/administrative-court-daily-cause-list/administrativeCourtDailyCauseList.xlsx
+++ b/src/integrationTest/resources/data/non-strategic/administrative-court-daily-cause-list/administrativeCourtDailyCauseList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junaid.iqbal/Documents/GitHub/pip-data-management/src/integrationTest/resources/data/non-strategic/birmingham-administrative-court-daily-cause-list/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junaid.iqbal/Documents/GitHub/pip-data-management/src/integrationTest/resources/data/non-strategic/administrative-court-daily-cause-list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C120808-23B8-5D49-A356-9B3FF5AA9E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D63D6F-6C02-944A-A13E-726D6858C7AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31640" yWindow="1640" windowWidth="27640" windowHeight="16940" xr2:uid="{0C1F814A-B1E5-C24D-AA62-DAE35072E02F}"/>
+    <workbookView xWindow="0" yWindow="2240" windowWidth="14400" windowHeight="9660" xr2:uid="{0C1F814A-B1E5-C24D-AA62-DAE35072E02F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>Additional Information</t>
   </si>
   <si>
-    <t>11am</t>
-  </si>
-  <si>
     <t>This is additional information</t>
   </si>
   <si>
@@ -86,13 +83,16 @@
     <t>Hearing Type</t>
   </si>
   <si>
-    <t>10am</t>
-  </si>
-  <si>
     <t>Directions A</t>
   </si>
   <si>
     <t>Directions B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10am           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:30pm                </t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,22 +485,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
       <c r="F1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -508,48 +508,48 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>12345</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <v>12346</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revert test file changes and fix build
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/data/non-strategic/administrative-court-daily-cause-list/administrativeCourtDailyCauseList.xlsx
+++ b/src/integrationTest/resources/data/non-strategic/administrative-court-daily-cause-list/administrativeCourtDailyCauseList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junaid.iqbal/Documents/GitHub/pip-data-management/src/integrationTest/resources/data/non-strategic/administrative-court-daily-cause-list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D63D6F-6C02-944A-A13E-726D6858C7AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FF46E7-F48A-EA44-A0C5-46F55C669190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2240" windowWidth="14400" windowHeight="9660" xr2:uid="{0C1F814A-B1E5-C24D-AA62-DAE35072E02F}"/>
   </bookViews>
@@ -89,10 +89,10 @@
     <t>Directions B</t>
   </si>
   <si>
-    <t xml:space="preserve">10am           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1:30pm                </t>
+    <t>10am</t>
+  </si>
+  <si>
+    <t>1:30pm</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
revert test file changes
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/data/non-strategic/administrative-court-daily-cause-list/administrativeCourtDailyCauseList.xlsx
+++ b/src/integrationTest/resources/data/non-strategic/administrative-court-daily-cause-list/administrativeCourtDailyCauseList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junaid.iqbal/Documents/GitHub/pip-data-management/src/integrationTest/resources/data/non-strategic/administrative-court-daily-cause-list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FF46E7-F48A-EA44-A0C5-46F55C669190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036CE72E-D576-D04B-A55F-17B937E73E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2240" windowWidth="14400" windowHeight="9660" xr2:uid="{0C1F814A-B1E5-C24D-AA62-DAE35072E02F}"/>
   </bookViews>
@@ -471,7 +471,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
PUB-2963 Allow space at the end of Time for non-strategic publications (#762)
* Allow spaces at the end of hearing time

* revert test file changes and fix build

* revert test file changes

---------

Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/data/non-strategic/administrative-court-daily-cause-list/administrativeCourtDailyCauseList.xlsx
+++ b/src/integrationTest/resources/data/non-strategic/administrative-court-daily-cause-list/administrativeCourtDailyCauseList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junaid.iqbal/Documents/GitHub/pip-data-management/src/integrationTest/resources/data/non-strategic/birmingham-administrative-court-daily-cause-list/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junaid.iqbal/Documents/GitHub/pip-data-management/src/integrationTest/resources/data/non-strategic/administrative-court-daily-cause-list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C120808-23B8-5D49-A356-9B3FF5AA9E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036CE72E-D576-D04B-A55F-17B937E73E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31640" yWindow="1640" windowWidth="27640" windowHeight="16940" xr2:uid="{0C1F814A-B1E5-C24D-AA62-DAE35072E02F}"/>
+    <workbookView xWindow="0" yWindow="2240" windowWidth="14400" windowHeight="9660" xr2:uid="{0C1F814A-B1E5-C24D-AA62-DAE35072E02F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>Additional Information</t>
   </si>
   <si>
-    <t>11am</t>
-  </si>
-  <si>
     <t>This is additional information</t>
   </si>
   <si>
@@ -86,13 +83,16 @@
     <t>Hearing Type</t>
   </si>
   <si>
+    <t>Directions A</t>
+  </si>
+  <si>
+    <t>Directions B</t>
+  </si>
+  <si>
     <t>10am</t>
   </si>
   <si>
-    <t>Directions A</t>
-  </si>
-  <si>
-    <t>Directions B</t>
+    <t>1:30pm</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,22 +485,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
       <c r="F1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -508,48 +508,48 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>12345</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <v>12346</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>